<commit_message>
final chat data added
</commit_message>
<xml_diff>
--- a/agg_lang.xlsx
+++ b/agg_lang.xlsx
@@ -733,7 +733,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -761,7 +761,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -985,7 +985,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1013,7 +1013,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1041,7 +1041,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1069,7 +1069,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1097,7 +1097,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1125,7 +1125,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1181,7 +1181,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1265,7 +1265,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1293,7 +1293,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1349,7 +1349,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1377,7 +1377,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1433,7 +1433,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -1461,7 +1461,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1517,7 +1517,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -1545,7 +1545,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -1573,7 +1573,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -1601,7 +1601,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -1741,7 +1741,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -1769,7 +1769,7 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -1825,7 +1825,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -1853,7 +1853,7 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -2077,7 +2077,7 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
@@ -2105,7 +2105,7 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
@@ -2161,7 +2161,7 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
@@ -2189,7 +2189,7 @@
         </is>
       </c>
       <c r="E63" t="n">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
@@ -2245,7 +2245,7 @@
         </is>
       </c>
       <c r="E65" t="n">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
@@ -2273,7 +2273,7 @@
         </is>
       </c>
       <c r="E66" t="n">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
@@ -2497,7 +2497,7 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
@@ -2525,7 +2525,7 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
@@ -2581,7 +2581,7 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
@@ -2609,7 +2609,7 @@
         </is>
       </c>
       <c r="E78" t="n">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
@@ -2665,7 +2665,7 @@
         </is>
       </c>
       <c r="E80" t="n">
-        <v>881</v>
+        <v>888</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
@@ -2693,7 +2693,7 @@
         </is>
       </c>
       <c r="E81" t="n">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
@@ -2749,7 +2749,7 @@
         </is>
       </c>
       <c r="E83" t="n">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
@@ -2777,7 +2777,7 @@
         </is>
       </c>
       <c r="E84" t="n">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
@@ -2833,7 +2833,7 @@
         </is>
       </c>
       <c r="E86" t="n">
-        <v>993</v>
+        <v>998</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
@@ -2861,7 +2861,7 @@
         </is>
       </c>
       <c r="E87" t="n">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
@@ -2917,7 +2917,7 @@
         </is>
       </c>
       <c r="E89" t="n">
-        <v>867</v>
+        <v>860</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
@@ -2945,7 +2945,7 @@
         </is>
       </c>
       <c r="E90" t="n">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
@@ -3001,7 +3001,7 @@
         </is>
       </c>
       <c r="E92" t="n">
-        <v>1099</v>
+        <v>1102</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
@@ -3029,7 +3029,7 @@
         </is>
       </c>
       <c r="E93" t="n">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
@@ -3085,7 +3085,7 @@
         </is>
       </c>
       <c r="E95" t="n">
-        <v>911</v>
+        <v>906</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
@@ -3113,7 +3113,7 @@
         </is>
       </c>
       <c r="E96" t="n">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
@@ -3169,7 +3169,7 @@
         </is>
       </c>
       <c r="E98" t="n">
-        <v>1154</v>
+        <v>1160</v>
       </c>
       <c r="F98" t="inlineStr">
         <is>
@@ -3197,7 +3197,7 @@
         </is>
       </c>
       <c r="E99" t="n">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
@@ -3253,7 +3253,7 @@
         </is>
       </c>
       <c r="E101" t="n">
-        <v>855</v>
+        <v>858</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
@@ -3281,7 +3281,7 @@
         </is>
       </c>
       <c r="E102" t="n">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F102" t="inlineStr">
         <is>
@@ -3337,7 +3337,7 @@
         </is>
       </c>
       <c r="E104" t="n">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="F104" t="inlineStr">
         <is>
@@ -3365,7 +3365,7 @@
         </is>
       </c>
       <c r="E105" t="n">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F105" t="inlineStr">
         <is>
@@ -3421,7 +3421,7 @@
         </is>
       </c>
       <c r="E107" t="n">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="F107" t="inlineStr">
         <is>
@@ -3449,7 +3449,7 @@
         </is>
       </c>
       <c r="E108" t="n">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="F108" t="inlineStr">
         <is>
@@ -3505,7 +3505,7 @@
         </is>
       </c>
       <c r="E110" t="n">
-        <v>1130</v>
+        <v>1115</v>
       </c>
       <c r="F110" t="inlineStr">
         <is>
@@ -3533,7 +3533,7 @@
         </is>
       </c>
       <c r="E111" t="n">
-        <v>428</v>
+        <v>443</v>
       </c>
       <c r="F111" t="inlineStr">
         <is>
@@ -3589,7 +3589,7 @@
         </is>
       </c>
       <c r="E113" t="n">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
@@ -3617,7 +3617,7 @@
         </is>
       </c>
       <c r="E114" t="n">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
@@ -3673,7 +3673,7 @@
         </is>
       </c>
       <c r="E116" t="n">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="F116" t="inlineStr">
         <is>
@@ -3701,7 +3701,7 @@
         </is>
       </c>
       <c r="E117" t="n">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="F117" t="inlineStr">
         <is>
@@ -3757,7 +3757,7 @@
         </is>
       </c>
       <c r="E119" t="n">
-        <v>966</v>
+        <v>969</v>
       </c>
       <c r="F119" t="inlineStr">
         <is>
@@ -3785,7 +3785,7 @@
         </is>
       </c>
       <c r="E120" t="n">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="F120" t="inlineStr">
         <is>
@@ -3841,7 +3841,7 @@
         </is>
       </c>
       <c r="E122" t="n">
-        <v>1246</v>
+        <v>1250</v>
       </c>
       <c r="F122" t="inlineStr">
         <is>
@@ -3869,7 +3869,7 @@
         </is>
       </c>
       <c r="E123" t="n">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="F123" t="inlineStr">
         <is>
@@ -3925,7 +3925,7 @@
         </is>
       </c>
       <c r="E125" t="n">
-        <v>946</v>
+        <v>941</v>
       </c>
       <c r="F125" t="inlineStr">
         <is>
@@ -3953,7 +3953,7 @@
         </is>
       </c>
       <c r="E126" t="n">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="F126" t="inlineStr">
         <is>
@@ -4093,7 +4093,7 @@
         </is>
       </c>
       <c r="E131" t="n">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="F131" t="inlineStr">
         <is>
@@ -4121,7 +4121,7 @@
         </is>
       </c>
       <c r="E132" t="n">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="F132" t="inlineStr">
         <is>
@@ -4177,7 +4177,7 @@
         </is>
       </c>
       <c r="E134" t="n">
-        <v>786</v>
+        <v>775</v>
       </c>
       <c r="F134" t="inlineStr">
         <is>
@@ -4205,7 +4205,7 @@
         </is>
       </c>
       <c r="E135" t="n">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="F135" t="inlineStr">
         <is>
@@ -4261,7 +4261,7 @@
         </is>
       </c>
       <c r="E137" t="n">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="F137" t="inlineStr">
         <is>
@@ -4289,7 +4289,7 @@
         </is>
       </c>
       <c r="E138" t="n">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="F138" t="inlineStr">
         <is>
@@ -4345,7 +4345,7 @@
         </is>
       </c>
       <c r="E140" t="n">
-        <v>912</v>
+        <v>925</v>
       </c>
       <c r="F140" t="inlineStr">
         <is>
@@ -4373,7 +4373,7 @@
         </is>
       </c>
       <c r="E141" t="n">
-        <v>525</v>
+        <v>512</v>
       </c>
       <c r="F141" t="inlineStr">
         <is>
@@ -4429,7 +4429,7 @@
         </is>
       </c>
       <c r="E143" t="n">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="F143" t="inlineStr">
         <is>
@@ -4457,7 +4457,7 @@
         </is>
       </c>
       <c r="E144" t="n">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F144" t="inlineStr">
         <is>
@@ -4513,7 +4513,7 @@
         </is>
       </c>
       <c r="E146" t="n">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="F146" t="inlineStr">
         <is>
@@ -4541,7 +4541,7 @@
         </is>
       </c>
       <c r="E147" t="n">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="F147" t="inlineStr">
         <is>
@@ -4597,7 +4597,7 @@
         </is>
       </c>
       <c r="E149" t="n">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="F149" t="inlineStr">
         <is>
@@ -4625,7 +4625,7 @@
         </is>
       </c>
       <c r="E150" t="n">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F150" t="inlineStr">
         <is>
@@ -4681,7 +4681,7 @@
         </is>
       </c>
       <c r="E152" t="n">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="F152" t="inlineStr">
         <is>
@@ -4709,7 +4709,7 @@
         </is>
       </c>
       <c r="E153" t="n">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="F153" t="inlineStr">
         <is>
@@ -4765,7 +4765,7 @@
         </is>
       </c>
       <c r="E155" t="n">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="F155" t="inlineStr">
         <is>
@@ -4793,7 +4793,7 @@
         </is>
       </c>
       <c r="E156" t="n">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="F156" t="inlineStr">
         <is>
@@ -4849,7 +4849,7 @@
         </is>
       </c>
       <c r="E158" t="n">
-        <v>845</v>
+        <v>850</v>
       </c>
       <c r="F158" t="inlineStr">
         <is>
@@ -4877,7 +4877,7 @@
         </is>
       </c>
       <c r="E159" t="n">
-        <v>852</v>
+        <v>847</v>
       </c>
       <c r="F159" t="inlineStr">
         <is>
@@ -4933,7 +4933,7 @@
         </is>
       </c>
       <c r="E161" t="n">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="F161" t="inlineStr">
         <is>
@@ -4961,7 +4961,7 @@
         </is>
       </c>
       <c r="E162" t="n">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="F162" t="inlineStr">
         <is>
@@ -5017,7 +5017,7 @@
         </is>
       </c>
       <c r="E164" t="n">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="F164" t="inlineStr">
         <is>
@@ -5045,7 +5045,7 @@
         </is>
       </c>
       <c r="E165" t="n">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="F165" t="inlineStr">
         <is>
@@ -5101,7 +5101,7 @@
         </is>
       </c>
       <c r="E167" t="n">
-        <v>751</v>
+        <v>755</v>
       </c>
       <c r="F167" t="inlineStr">
         <is>
@@ -5129,7 +5129,7 @@
         </is>
       </c>
       <c r="E168" t="n">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F168" t="inlineStr">
         <is>
@@ -5185,7 +5185,7 @@
         </is>
       </c>
       <c r="E170" t="n">
-        <v>954</v>
+        <v>967</v>
       </c>
       <c r="F170" t="inlineStr">
         <is>
@@ -5213,7 +5213,7 @@
         </is>
       </c>
       <c r="E171" t="n">
-        <v>510</v>
+        <v>497</v>
       </c>
       <c r="F171" t="inlineStr">
         <is>
@@ -5269,7 +5269,7 @@
         </is>
       </c>
       <c r="E173" t="n">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="F173" t="inlineStr">
         <is>
@@ -5297,7 +5297,7 @@
         </is>
       </c>
       <c r="E174" t="n">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="F174" t="inlineStr">
         <is>
@@ -5353,7 +5353,7 @@
         </is>
       </c>
       <c r="E176" t="n">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="F176" t="inlineStr">
         <is>
@@ -5381,7 +5381,7 @@
         </is>
       </c>
       <c r="E177" t="n">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="F177" t="inlineStr">
         <is>
@@ -5521,7 +5521,7 @@
         </is>
       </c>
       <c r="E182" t="n">
-        <v>613</v>
+        <v>603</v>
       </c>
       <c r="F182" t="inlineStr">
         <is>
@@ -5549,7 +5549,7 @@
         </is>
       </c>
       <c r="E183" t="n">
-        <v>502</v>
+        <v>512</v>
       </c>
       <c r="F183" t="inlineStr">
         <is>
@@ -5605,7 +5605,7 @@
         </is>
       </c>
       <c r="E185" t="n">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="F185" t="inlineStr">
         <is>
@@ -5633,7 +5633,7 @@
         </is>
       </c>
       <c r="E186" t="n">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="F186" t="inlineStr">
         <is>
@@ -5689,7 +5689,7 @@
         </is>
       </c>
       <c r="E188" t="n">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="F188" t="inlineStr">
         <is>
@@ -5717,7 +5717,7 @@
         </is>
       </c>
       <c r="E189" t="n">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="F189" t="inlineStr">
         <is>
@@ -5773,7 +5773,7 @@
         </is>
       </c>
       <c r="E191" t="n">
-        <v>635</v>
+        <v>645</v>
       </c>
       <c r="F191" t="inlineStr">
         <is>
@@ -5801,7 +5801,7 @@
         </is>
       </c>
       <c r="E192" t="n">
-        <v>508</v>
+        <v>498</v>
       </c>
       <c r="F192" t="inlineStr">
         <is>
@@ -5857,7 +5857,7 @@
         </is>
       </c>
       <c r="E194" t="n">
-        <v>857</v>
+        <v>850</v>
       </c>
       <c r="F194" t="inlineStr">
         <is>
@@ -5885,7 +5885,7 @@
         </is>
       </c>
       <c r="E195" t="n">
-        <v>635</v>
+        <v>642</v>
       </c>
       <c r="F195" t="inlineStr">
         <is>
@@ -5941,7 +5941,7 @@
         </is>
       </c>
       <c r="E197" t="n">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="F197" t="inlineStr">
         <is>
@@ -5969,7 +5969,7 @@
         </is>
       </c>
       <c r="E198" t="n">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="F198" t="inlineStr">
         <is>
@@ -6025,7 +6025,7 @@
         </is>
       </c>
       <c r="E200" t="n">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="F200" t="inlineStr">
         <is>
@@ -6053,7 +6053,7 @@
         </is>
       </c>
       <c r="E201" t="n">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="F201" t="inlineStr">
         <is>
@@ -6109,7 +6109,7 @@
         </is>
       </c>
       <c r="E203" t="n">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F203" t="inlineStr">
         <is>
@@ -6137,7 +6137,7 @@
         </is>
       </c>
       <c r="E204" t="n">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F204" t="inlineStr">
         <is>
@@ -6193,7 +6193,7 @@
         </is>
       </c>
       <c r="E206" t="n">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="F206" t="inlineStr">
         <is>
@@ -6221,7 +6221,7 @@
         </is>
       </c>
       <c r="E207" t="n">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="F207" t="inlineStr">
         <is>
@@ -6277,7 +6277,7 @@
         </is>
       </c>
       <c r="E209" t="n">
-        <v>411</v>
+        <v>588</v>
       </c>
       <c r="F209" t="inlineStr">
         <is>
@@ -6305,7 +6305,7 @@
         </is>
       </c>
       <c r="E210" t="n">
-        <v>471</v>
+        <v>811</v>
       </c>
       <c r="F210" t="inlineStr">
         <is>
@@ -6333,7 +6333,7 @@
         </is>
       </c>
       <c r="E211" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F211" t="inlineStr">
         <is>
@@ -6361,7 +6361,7 @@
         </is>
       </c>
       <c r="E212" t="n">
-        <v>501</v>
+        <v>744</v>
       </c>
       <c r="F212" t="inlineStr">
         <is>
@@ -6389,7 +6389,7 @@
         </is>
       </c>
       <c r="E213" t="n">
-        <v>583</v>
+        <v>1028</v>
       </c>
       <c r="F213" t="inlineStr">
         <is>
@@ -6417,7 +6417,7 @@
         </is>
       </c>
       <c r="E214" t="n">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="F214" t="inlineStr">
         <is>

</xml_diff>